<commit_message>
[svn r83] Moved csv/xls/xlsx functionality into separate modules. Pylint, lots of comments, removing dead code, and refactoring. Started using Bunch(), a dynamic struct.
--HG--
branch : trunk
</commit_message>
<xml_diff>
--- a/blueprints/Tests/proper-size.xlsx
+++ b/blueprints/Tests/proper-size.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="9">
   <si>
     <t>d</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>gray box defines the expected first layer size; yellow box defines the expected second layer size.</t>
+  </si>
+  <si>
+    <t>all # symbols should get ignored</t>
+  </si>
+  <si>
+    <t>x(3x1)</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="17.25" customHeight="1"/>
@@ -463,11 +469,10 @@
       <c r="G5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="I5" s="1"/>
-      <c r="L5" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="6" spans="1:12" ht="17.25" customHeight="1">
       <c r="A6" s="1"/>
@@ -510,61 +515,132 @@
     <row r="8" spans="1:12" ht="17.25" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>3</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>5</v>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="17.25" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="17.25" customHeight="1">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" ht="17.25" customHeight="1">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>5</v>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="17.25" customHeight="1">
-      <c r="B12" t="s">
-        <v>5</v>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="17.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="17.25" customHeight="1">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="17.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="17.25" customHeight="1">
+      <c r="B17" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>